<commit_message>
Modified planning burndown chart to fix mistake. Added the actual execution for sprint0
</commit_message>
<xml_diff>
--- a/Sprint0/Planning and Burndown/Initial Plan and Burndown Chart.xlsx
+++ b/Sprint0/Planning and Burndown/Initial Plan and Burndown Chart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qi\Desktop\Team27\Team27\Sprint0\Planning and Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC11B33D-502F-42CA-B387-D85755E6103D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE5D94D-C6B1-46F6-9AD2-CABD795CC805}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4530" xr2:uid="{BA48CDB0-28D6-40BA-AC4E-2E3225A2E410}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4530" activeTab="1" xr2:uid="{BA48CDB0-28D6-40BA-AC4E-2E3225A2E410}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="57">
   <si>
     <t>Column1</t>
   </si>
@@ -193,9 +193,6 @@
   </si>
   <si>
     <t>T:2</t>
-  </si>
-  <si>
-    <t>v</t>
   </si>
   <si>
     <t>Days</t>
@@ -396,9 +393,8 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> for Sprint 1</a:t>
+              <a:t> for Sprint 0</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -1500,17 +1496,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5D3AD17F-A853-466D-A9CA-12E05E908158}" name="plan" displayName="plan" ref="A1:K23" tableType="queryTable" totalsRowCount="1">
   <autoFilter ref="A1:K22" xr:uid="{00060DD0-BAC4-49DB-B777-2AD51945B21C}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E6A67218-65C3-450E-981F-C5D0DDFECB80}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="20" totalsRowDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{01A729D2-CB83-4525-9D9B-E1672D1DFB51}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="18" totalsRowDxfId="19"/>
-    <tableColumn id="3" xr3:uid="{F17DFA1C-E5B1-4491-9158-17E052CD8E86}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="16" totalsRowDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{D1EF87E4-CC7A-4199-862E-DE742B71040C}" uniqueName="4" name="Column4" totalsRowFunction="sum" queryTableFieldId="4" dataDxfId="14" totalsRowDxfId="15"/>
-    <tableColumn id="5" xr3:uid="{921F0D27-66F4-4866-A00F-61D221E6BBF5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="12" totalsRowDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{F28DF117-B94E-453D-BD75-FDB2AD09A1BE}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="10" totalsRowDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{2CE7BDFE-F433-4E62-B93E-6CE74883CC0B}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{EC6DC6FE-472E-4184-B0D4-A9DB2DBAA9BC}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="6" totalsRowDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{3B482E12-163F-418C-B548-D484AE3F1750}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="4" totalsRowDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{69C35119-DF90-413B-810E-DD34C8AAAE0A}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{ED857004-AD81-47D6-A573-4C0086DE790E}" uniqueName="12" name="Column11" queryTableFieldId="12" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{E6A67218-65C3-450E-981F-C5D0DDFECB80}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{01A729D2-CB83-4525-9D9B-E1672D1DFB51}" uniqueName="2" name="Column2" queryTableFieldId="2" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{F17DFA1C-E5B1-4491-9158-17E052CD8E86}" uniqueName="3" name="Column3" queryTableFieldId="3" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="4" xr3:uid="{D1EF87E4-CC7A-4199-862E-DE742B71040C}" uniqueName="4" name="Column4" totalsRowFunction="sum" queryTableFieldId="4" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{921F0D27-66F4-4866-A00F-61D221E6BBF5}" uniqueName="5" name="Column5" queryTableFieldId="5" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{F28DF117-B94E-453D-BD75-FDB2AD09A1BE}" uniqueName="6" name="Column6" queryTableFieldId="6" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{2CE7BDFE-F433-4E62-B93E-6CE74883CC0B}" uniqueName="7" name="Column7" queryTableFieldId="7" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="8" xr3:uid="{EC6DC6FE-472E-4184-B0D4-A9DB2DBAA9BC}" uniqueName="8" name="Column8" queryTableFieldId="8" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{3B482E12-163F-418C-B548-D484AE3F1750}" uniqueName="9" name="Column9" queryTableFieldId="9" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{69C35119-DF90-413B-810E-DD34C8AAAE0A}" uniqueName="10" name="Column10" queryTableFieldId="10" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="12" xr3:uid="{ED857004-AD81-47D6-A573-4C0086DE790E}" uniqueName="12" name="Column11" queryTableFieldId="12" dataDxfId="2" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1520,7 +1516,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{DCD7645C-5F70-4B0C-B8D3-88B8CD1739BD}" name="burndown" displayName="burndown" ref="A1:I5" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:I5" xr:uid="{A449F7A1-CA1F-42BE-B714-D5143C1D5D65}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{8F51A259-8249-48C1-9971-91797E058838}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{8F51A259-8249-48C1-9971-91797E058838}" uniqueName="1" name="Column1" queryTableFieldId="1" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{D5B70BF6-CBD6-4E0B-8C9B-EDFCE4802C8F}" uniqueName="2" name="Column2" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{46BD4B7D-9D5E-4074-B41E-C1520BD18404}" uniqueName="3" name="Column3" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{B7A537DB-E075-49B8-A739-05D9408C0620}" uniqueName="4" name="Column4" queryTableFieldId="4"/>
@@ -1833,8 +1829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B413779-8E14-4591-97B7-D61D7FA0B81F}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1946,7 +1942,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1976,7 +1972,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2002,7 +1998,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2026,7 +2022,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2050,7 +2046,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2423,8 +2419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C1A0DD3-4C7F-400B-AA76-48F9032ADAB6}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2463,13 +2459,11 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>49</v>
-      </c>
+      <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2498,7 +2492,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4">
         <v>55</v>
@@ -2527,7 +2521,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5">
         <v>55</v>

</xml_diff>